<commit_message>
fix: pequeños ajustes y correcciones
</commit_message>
<xml_diff>
--- a/backend/Reporte Plantilla.xlsx
+++ b/backend/Reporte Plantilla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Zonagamer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Zonagamer\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A73A68-A86B-4987-A71D-AC1297902C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACB5517-79DA-46C9-B051-04C5CAA047AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{AA21D85A-83E0-456A-9149-1789D8CD4271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA21D85A-83E0-456A-9149-1789D8CD4271}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Reporte del día:</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Tiempo</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +541,7 @@
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -697,25 +701,28 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>